<commit_message>
favorite items and product in category
</commit_message>
<xml_diff>
--- a/MurrayaEcomAdminModuleScreenFlow.xlsx
+++ b/MurrayaEcomAdminModuleScreenFlow.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ecommerce\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ecommerce\murraya_ecommerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E194081-5959-4464-BAD9-294EEB523833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E48A32-3C20-4A62-BD17-B31C5B8CF1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A9E55622-9D36-435C-B6F2-F42FACD478B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="8" xr2:uid="{A9E55622-9D36-435C-B6F2-F42FACD478B6}"/>
   </bookViews>
   <sheets>
     <sheet name="screen_flow" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,8 @@
     <sheet name="5. Order Management" sheetId="6" r:id="rId6"/>
     <sheet name="6. User Management" sheetId="7" r:id="rId7"/>
     <sheet name="7. Product Reviews" sheetId="9" r:id="rId8"/>
-    <sheet name="status" sheetId="2" r:id="rId9"/>
+    <sheet name="8.Product Discounts" sheetId="10" r:id="rId9"/>
+    <sheet name="status" sheetId="2" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="93">
   <si>
     <t>B. Admin Journey (Back Office)</t>
   </si>
@@ -270,6 +271,48 @@
   </si>
   <si>
     <t>Review Management</t>
+  </si>
+  <si>
+    <t>Product Discount Management</t>
+  </si>
+  <si>
+    <t>/admin/discountManagement</t>
+  </si>
+  <si>
+    <t>/admin/discounts/apply</t>
+  </si>
+  <si>
+    <t>/admin/discounts/applyDiscount</t>
+  </si>
+  <si>
+    <t>/admin/discounts/removeDiscount</t>
+  </si>
+  <si>
+    <t>/admin/discounts/addDiscount</t>
+  </si>
+  <si>
+    <t>/admin/discounts/updateDiscount/{discountId}</t>
+  </si>
+  <si>
+    <t>/admin/discounts/deleteDiscount/{discountId}</t>
+  </si>
+  <si>
+    <t>/admin/discounts//viewDiscount/{discountId}</t>
+  </si>
+  <si>
+    <t>Discounts apply/remove to product</t>
+  </si>
+  <si>
+    <t>Create discount</t>
+  </si>
+  <si>
+    <t>Update discount</t>
+  </si>
+  <si>
+    <t>Delete discount</t>
+  </si>
+  <si>
+    <t>View discount</t>
   </si>
 </sst>
 </file>
@@ -381,7 +424,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -476,11 +519,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -531,6 +585,9 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -552,14 +609,20 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -882,7 +945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32886694-956E-4440-B04F-818BC7487BE3}">
   <dimension ref="B5:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -893,18 +956,18 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
     </row>
     <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -1048,12 +1111,98 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ACDD1C6-EF67-4E8B-BF80-A5EFD2523DA3}">
+  <dimension ref="B3:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C6" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C6:F6"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:F8" xr:uid="{A795B99E-0905-4DBA-9926-65660A3F80F3}">
+      <formula1>$B$3:$B$5</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B984A8B-5488-4F7F-8630-D7A41BD996E5}">
   <dimension ref="B5:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,12 +1213,12 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -1167,7 +1316,7 @@
   <dimension ref="B4:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,12 +1328,12 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -1300,12 +1449,12 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
@@ -1426,12 +1575,12 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
@@ -1637,12 +1786,12 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
@@ -1731,12 +1880,12 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
@@ -1753,7 +1902,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="20" t="s">
         <v>48</v>
       </c>
       <c r="C6" s="19" t="s">
@@ -1883,7 +2032,7 @@
   <dimension ref="C5:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1894,12 +2043,12 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
     </row>
     <row r="6" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="8" t="s">
@@ -1916,10 +2065,10 @@
       </c>
     </row>
     <row r="7" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="6" t="s">
         <v>75</v>
       </c>
       <c r="E7" s="7" t="s">
@@ -1933,7 +2082,7 @@
       <c r="C8" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="6" t="s">
         <v>76</v>
       </c>
       <c r="E8" s="7" t="s">
@@ -1945,7 +2094,7 @@
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" s="29"/>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="6" t="s">
         <v>77</v>
       </c>
       <c r="E9" s="7" t="s">
@@ -2001,87 +2150,167 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ACDD1C6-EF67-4E8B-BF80-A5EFD2523DA3}">
-  <dimension ref="B3:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A60A09E-B988-4D80-9C63-DE944052211E}">
+  <dimension ref="C6:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C6" s="23" t="s">
+    <row r="6" spans="3:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C6" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="11" t="s">
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+    </row>
+    <row r="7" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C7" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="2" t="s">
-        <v>65</v>
+    <row r="8" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C8" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>10</v>
+        <v>80</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="31"/>
+      <c r="D10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="32"/>
+      <c r="D11" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C12" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C13" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C14" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C15" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C9:C11"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:F8" xr:uid="{A795B99E-0905-4DBA-9926-65660A3F80F3}">
-      <formula1>$B$3:$B$5</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{315497D5-DAD3-44D1-AC32-E59BEB8FB974}">
+          <x14:formula1>
+            <xm:f>status!$B$3:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E8:F15</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>